<commit_message>
Services done and api program.cs is configured as is appsetting almost
</commit_message>
<xml_diff>
--- a/Tidsplan.xlsx
+++ b/Tidsplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{A0747018-251B-49C7-9A7B-C7C717FFACA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AC17F39-1EEA-4849-8D5E-F2539B7370EC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F62804-50C6-4F4E-84E9-CFA2FA06106C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1129,10 +1129,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1366,8 +1362,8 @@
   </sheetPr>
   <dimension ref="B1:BH28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1953,7 +1949,7 @@
         <v>7</v>
       </c>
       <c r="F12" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="4">
         <v>1</v>
@@ -2030,7 +2026,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="18">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F14" s="18">
         <v>1</v>
@@ -2597,20 +2593,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb3db277-d37c-4294-a18a-6883eecb93af" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb3db277-d37c-4294-a18a-6883eecb93af" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2867,19 +2863,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{787DBAEB-0AF3-4324-B644-BA0D2DE78C72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F279105-63CB-4F93-BBA6-A58E9F83F048}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="fb3db277-d37c-4294-a18a-6883eecb93af"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{787DBAEB-0AF3-4324-B644-BA0D2DE78C72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Controllers and light testing
</commit_message>
<xml_diff>
--- a/Tidsplan.xlsx
+++ b/Tidsplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F62804-50C6-4F4E-84E9-CFA2FA06106C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7511D88D-A1AE-48B5-A619-DC9592209D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1363,7 +1363,7 @@
   <dimension ref="B1:BH28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2066,7 +2066,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="18">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F15" s="18">
         <v>1</v>
@@ -2593,23 +2593,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb3db277-d37c-4294-a18a-6883eecb93af" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101007C4BF558AE40D240BDDA30BBA5DAD0CC" ma:contentTypeVersion="18" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="2423199d00ac53f4531f05361a1af8e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="02c16ba3-7f80-451e-a59f-75dc6b30dc03" xmlns:ns4="fb3db277-d37c-4294-a18a-6883eecb93af" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd2e8d830613da71b7c051ecf8052be6" ns3:_="" ns4:_="">
     <xsd:import namespace="02c16ba3-7f80-451e-a59f-75dc6b30dc03"/>
@@ -2862,25 +2845,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{787DBAEB-0AF3-4324-B644-BA0D2DE78C72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb3db277-d37c-4294-a18a-6883eecb93af" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F279105-63CB-4F93-BBA6-A58E9F83F048}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb3db277-d37c-4294-a18a-6883eecb93af"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3CF3D8E-CC0D-41DE-8CA4-E0739BBF2CD7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2897,4 +2879,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F279105-63CB-4F93-BBA6-A58E9F83F048}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb3db277-d37c-4294-a18a-6883eecb93af"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{787DBAEB-0AF3-4324-B644-BA0D2DE78C72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Login and register pages
</commit_message>
<xml_diff>
--- a/Tidsplan.xlsx
+++ b/Tidsplan.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7511D88D-A1AE-48B5-A619-DC9592209D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CF2D74-8E8B-4BFB-B2DD-49CD3CA79307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1363,7 +1363,7 @@
   <dimension ref="B1:BH28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2106,10 +2106,10 @@
         <v>1</v>
       </c>
       <c r="E16" s="18">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F16" s="18">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G16" s="4">
         <v>0.75</v>
@@ -2146,7 +2146,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="18">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F17" s="18">
         <v>1</v>
@@ -2593,6 +2593,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb3db277-d37c-4294-a18a-6883eecb93af" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101007C4BF558AE40D240BDDA30BBA5DAD0CC" ma:contentTypeVersion="18" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="2423199d00ac53f4531f05361a1af8e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="02c16ba3-7f80-451e-a59f-75dc6b30dc03" xmlns:ns4="fb3db277-d37c-4294-a18a-6883eecb93af" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd2e8d830613da71b7c051ecf8052be6" ns3:_="" ns4:_="">
     <xsd:import namespace="02c16ba3-7f80-451e-a59f-75dc6b30dc03"/>
@@ -2845,24 +2862,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb3db277-d37c-4294-a18a-6883eecb93af" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{787DBAEB-0AF3-4324-B644-BA0D2DE78C72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F279105-63CB-4F93-BBA6-A58E9F83F048}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb3db277-d37c-4294-a18a-6883eecb93af"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3CF3D8E-CC0D-41DE-8CA4-E0739BBF2CD7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2879,22 +2897,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F279105-63CB-4F93-BBA6-A58E9F83F048}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb3db277-d37c-4294-a18a-6883eecb93af"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{787DBAEB-0AF3-4324-B644-BA0D2DE78C72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>